<commit_message>
release mCSD 3.8.0 to TI
</commit_message>
<xml_diff>
--- a/ITI/mCSD/CodeSystem-mcsd-example-hierarchy.xlsx
+++ b/ITI/mCSD/CodeSystem-mcsd-example-hierarchy.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.5.0</t>
+    <t>3.8.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-02-28T19:51:02-06:00</t>
+    <t>2022-08-12T09:44:57-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Copyright</t>
-  </si>
-  <si>
-    <t>IHE http://www.ihe.net/Governance/#Intellectual_Property</t>
   </si>
   <si>
     <t>Case Sensitive</t>
@@ -419,62 +416,60 @@
       <c r="A16" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="B16" t="s" s="2">
-        <v>26</v>
-      </c>
+      <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s" s="2">
         <v>27</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>33</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>34</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s" s="2">
         <v>36</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -492,39 +487,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>38</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>39</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>40</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>43</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="2">
         <v>45</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>46</v>
       </c>
       <c r="D3" s="2"/>
     </row>

</xml_diff>